<commit_message>
Problem statement changed a bit
</commit_message>
<xml_diff>
--- a/Problem_statement.xlsx
+++ b/Problem_statement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srahu\OneDrive\Desktop\SQL_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0409D398-D86F-4D45-927D-6854CBF4C961}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401740B5-380F-4B96-A346-A55581298886}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{D880422C-F7CE-4A8A-8F11-88FD68F210C3}"/>
   </bookViews>
@@ -45,12 +45,6 @@
     <t>Total Cases Vs Total Deaths per Country</t>
   </si>
   <si>
-    <t>Highest Covid Infected Cases per country(location)</t>
-  </si>
-  <si>
-    <t>Highest Motality Count due to Covid per country(location)</t>
-  </si>
-  <si>
     <t>Highest Motality percent due to Covid per population</t>
   </si>
   <si>
@@ -60,10 +54,16 @@
     <t>Total count of people in the world who is vaccinated</t>
   </si>
   <si>
-    <t>Vaccination by running total per country(location)</t>
-  </si>
-  <si>
-    <t>Percentage for Running total of Vaccinated Vs Population per country(location)</t>
+    <t>Highest Covid Infected Cases per country(Locations)</t>
+  </si>
+  <si>
+    <t>Highest Motality Count due to Covid per country(Locations)</t>
+  </si>
+  <si>
+    <t>Vaccination by running total per country(Locations)</t>
+  </si>
+  <si>
+    <t>Percentage for Running total of Vaccinated Vs Population per country(Locations)</t>
   </si>
 </sst>
 </file>
@@ -435,7 +435,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,27 +480,27 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>